<commit_message>
Day 8 | Initial Commit
</commit_message>
<xml_diff>
--- a/Batch/14/Curriculum/Day_8_Error.xlsx
+++ b/Batch/14/Curriculum/Day_8_Error.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sunstone\Desktop\accio\Excel\Class Curriculum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\14\Curriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E15A2BD-B234-41A6-8D7D-FEB4C8F67B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E6F4F7-FB94-4F19-A045-9C0DC6746567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="750" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#NA" sheetId="1" r:id="rId1"/>
@@ -325,15 +325,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -343,16 +361,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -361,25 +376,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -667,26 +667,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="H1" s="25" t="s">
+    <row r="1" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="H1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-    </row>
-    <row r="4" spans="3:11" ht="16" x14ac:dyDescent="0.5">
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="4" spans="3:11" ht="16.149999999999999" x14ac:dyDescent="0.65">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
@@ -694,85 +694,85 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="12"/>
-    </row>
-    <row r="8" spans="3:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="3:11" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="4">
         <v>23</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="1" t="e">
+      <c r="H8" s="15" t="e">
         <f>VLOOKUP(G8,$C$7:$D$12,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="4">
         <v>43</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="4">
         <v>54</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="4">
         <v>54</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
@@ -797,27 +797,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08775173-5547-48C4-86EC-BB7A6386EF27}">
   <dimension ref="C1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I7" sqref="I7:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="H1" s="25" t="s">
+    <row r="1" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="H1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-    </row>
-    <row r="4" spans="3:11" ht="16" x14ac:dyDescent="0.5">
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="4" spans="3:11" ht="16.149999999999999" x14ac:dyDescent="0.65">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
@@ -825,107 +825,107 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="3:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="C7" s="9" t="s">
+    <row r="7" spans="3:11" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-    </row>
-    <row r="8" spans="3:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="7">
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="3:11" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="1">
         <v>3310</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="1">
         <v>50</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="1">
         <f>C8/D8</f>
         <v>66.2</v>
       </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-    </row>
-    <row r="9" spans="3:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="C9" s="7">
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+    </row>
+    <row r="9" spans="3:11" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="C9" s="1">
         <v>1220</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="E9" s="7" t="e">
+      <c r="E9" s="1" t="e">
         <f t="shared" ref="E9:E12" si="0">C9/D9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C10" s="7">
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C10" s="1">
         <v>4440</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="1">
         <v>24</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>185</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C11" s="7">
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C11" s="1">
         <v>2301</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="1">
         <v>30</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="1">
         <f t="shared" si="0"/>
         <v>76.7</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C12" s="7">
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C12" s="1">
         <v>2222</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="1">
         <v>20</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>111.1</v>
       </c>
@@ -952,23 +952,23 @@
       <selection activeCell="H1" sqref="H1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="H1" s="25" t="s">
+    <row r="1" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="H1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-    </row>
-    <row r="4" spans="3:10" ht="16" x14ac:dyDescent="0.5">
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="4" spans="3:10" ht="16.149999999999999" x14ac:dyDescent="0.65">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
@@ -976,51 +976,51 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.45">
       <c r="D7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" spans="3:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="7">
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="3:10" ht="48" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="7" t="e">
+      <c r="G8" s="1" t="e">
         <f>D11+D10+D9+D8</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="D9" s="7">
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="D9" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="D10" s="7">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="D10" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="D11" s="7" t="s">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1043,23 +1043,23 @@
       <selection activeCell="H1" sqref="H1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="6" max="6" width="11.08984375" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.06640625" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="H1" s="25" t="s">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="H1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-    </row>
-    <row r="4" spans="3:9" ht="16" x14ac:dyDescent="0.5">
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="4" spans="3:9" ht="16.149999999999999" x14ac:dyDescent="0.65">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1067,19 +1067,19 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="3:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="D7" s="9" t="s">
+    <row r="7" spans="3:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="23"/>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.45">
       <c r="D8" s="4">
         <v>3310</v>
       </c>
@@ -1087,12 +1087,12 @@
         <f>D8/#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.45">
       <c r="D9" s="4">
         <v>1220</v>
       </c>
@@ -1100,10 +1100,10 @@
         <f>D9/#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.45">
       <c r="D10" s="4">
         <v>4440</v>
       </c>
@@ -1111,10 +1111,10 @@
         <f>D10/#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.45">
       <c r="D11" s="4">
         <v>2301</v>
       </c>
@@ -1122,10 +1122,10 @@
         <f>D11/#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.45">
       <c r="D12" s="4">
         <v>2222</v>
       </c>
@@ -1133,8 +1133,8 @@
         <f>D12/#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1155,25 +1155,25 @@
       <selection activeCell="H1" sqref="H1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="6" max="6" width="11.08984375" customWidth="1"/>
-    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.06640625" customWidth="1"/>
+    <col min="9" max="9" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.53125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="H1" s="25" t="s">
+    <row r="1" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="H1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-    </row>
-    <row r="4" spans="3:14" ht="16" x14ac:dyDescent="0.5">
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="4" spans="3:14" ht="16.149999999999999" x14ac:dyDescent="0.65">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1181,92 +1181,92 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.45">
       <c r="D7" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="L7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-    </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.45">
       <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="4">
         <v>22</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="J8" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="1" t="e" cm="1">
+      <c r="K8" s="15" t="e" cm="1">
         <f t="array" aca="1" ref="K8" ca="1">VLOKUP(I8,$D$7:$E$11,2,FALSE)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-    </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.45">
       <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="4">
         <v>554</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-    </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="I9" s="15"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.45">
       <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="4">
         <v>32</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-    </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="I10" s="15"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.45">
       <c r="D11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="4">
         <v>65</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1290,25 +1290,25 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="6" max="6" width="11.08984375" customWidth="1"/>
-    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.06640625" customWidth="1"/>
+    <col min="9" max="9" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.53125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="H1" s="25" t="s">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="H1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-    </row>
-    <row r="4" spans="3:9" ht="16" x14ac:dyDescent="0.5">
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="4" spans="3:9" ht="16.149999999999999" x14ac:dyDescent="0.65">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1316,46 +1316,46 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="D8" s="18" t="s">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="D8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-    </row>
-    <row r="9" spans="3:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="3:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D9" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="1" t="e">
+      <c r="E9" s="15" t="e">
         <f>187^549</f>
         <v>#NUM!</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.45">
       <c r="D10" s="26"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="E10" s="15"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.45">
       <c r="D11" s="26"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>